<commit_message>
further  writing of VAE implementation chapter
</commit_message>
<xml_diff>
--- a/LaTeX/data/variational autoencoder/PLOT_cost_per_epoch.xlsx
+++ b/LaTeX/data/variational autoencoder/PLOT_cost_per_epoch.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game Development\MasterThesis\Prototypte branch\TensorFlow Playground\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game Development\MasterThesis\LaTeX branch\LaTeX\data\variational autoencoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{796341D9-A113-449B-B432-FF29236725D8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EDD39756-36C0-4E91-A46B-C5E8D79853B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,62 +586,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
-                <a:ea typeface="+mj-ea"/>
-                <a:cs typeface="+mj-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Training Cost per Epoch</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1965,6 +1910,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1000"/>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1000" baseline="0"/>
+                  <a:t> Epoch</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT" sz="1000"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1988,7 +1993,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
@@ -2012,8 +2017,8 @@
         <c:axId val="343971663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
-          <c:min val="3"/>
+          <c:max val="18"/>
+          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2031,6 +2036,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1000"/>
+                  <a:t>Cost</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1000" baseline="0"/>
+                  <a:t> per Epoch</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2054,7 +2118,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
@@ -2763,9 +2827,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3093,7 +3157,7 @@
   <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>